<commit_message>
update test and embedding function
</commit_message>
<xml_diff>
--- a/recognition_log.xlsx
+++ b/recognition_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-12-02 10:22:07</t>
+          <t>2024-12-03 16:31:08</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -470,12 +470,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-12-02 10:22:40</t>
+          <t>2024-12-03 16:31:25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -487,29 +487,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-12-02 10:24:28</t>
+          <t>2024-12-03 16:31:38</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15/15 (100.00%)</t>
+          <t>11/15 (73.33%)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-12-02 10:25:03</t>
+          <t>2024-12-03 16:31:54</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-12-02 10:25:20</t>
+          <t>2024-12-03 16:32:13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9/15 (60.00%)</t>
+          <t>6/15 (40.00%)</t>
         </is>
       </c>
     </row>
@@ -543,41 +543,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-12-02 10:26:14</t>
+          <t>2024-12-03 16:32:24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14/15 (93.33%)</t>
+          <t>2/15 (13.33%)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>baejun</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-12-02 10:26:30</t>
+          <t>2024-12-03 16:33:06</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12/15 (80.00%)</t>
+          <t>0/15 (0.00%)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Quang lê</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-12-02 10:26:45</t>
+          <t>2024-12-03 16:33:16</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -589,51 +589,51 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>baejun</t>
+          <t>Quang lê</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-12-02 10:26:57</t>
+          <t>2024-12-03 16:33:33</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>15/15 (100.00%)</t>
+          <t>14/15 (93.33%)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DinhNhatKy</t>
+          <t>Quang lê</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-12-02 10:41:50</t>
+          <t>2024-12-03 16:33:57</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16/16 (100.00%)</t>
+          <t>15/15 (100.00%)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DinhNhatKy</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-12-02 10:42:08</t>
+          <t>2024-12-03 16:34:16</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16/16 (100.00%)</t>
+          <t>12/15 (80.00%)</t>
         </is>
       </c>
     </row>
@@ -645,80 +645,80 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-12-02 10:42:44</t>
+          <t>2024-12-03 16:34:30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16/16 (100.00%)</t>
+          <t>15/15 (100.00%)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DinhNhatKy</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-12-02 10:43:09</t>
+          <t>2024-12-03 16:34:40</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>16/16 (100.00%)</t>
+          <t>13/15 (86.67%)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DinhNhatKy</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-12-02 10:43:28</t>
+          <t>2024-12-03 16:34:53</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>16/16 (100.00%)</t>
+          <t>14/15 (93.33%)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DinhNhatKy</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-12-02 11:44:13</t>
+          <t>2024-12-03 16:35:11</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>15/15 (100.00%)</t>
+          <t>6/15 (40.00%)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>baejun</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-12-02 11:44:26</t>
+          <t>2024-12-03 16:35:32</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14/15 (93.33%)</t>
+          <t>15/15 (100.00%)</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-12-02 11:44:38</t>
+          <t>2024-12-03 16:35:44</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -742,12 +742,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>chipu</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-12-02 11:44:55</t>
+          <t>2024-12-03 16:35:54</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -759,12 +759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>sontung</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-12-02 11:45:14</t>
+          <t>2024-12-03 16:36:05</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,29 +781,556 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-12-02 11:45:35</t>
+          <t>2024-12-03 16:37:24</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14/15 (93.33%)</t>
+          <t>15/15 (100.00%)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>thaotam</t>
+          <t>DinhNhatKy</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-12-02 11:45:53</t>
+          <t>2024-12-03 16:37:38</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>13/15 (86.67%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Anh Hung</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:38:04</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Anh Hung</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:38:44</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>chipu</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:40:06</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:41:18</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:41:28</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:41:42</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>DinhNhatKy</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:47:13</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DinhNhatKy</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:47:25</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>DinhNhatKy</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:47:37</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>14/15 (93.33%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:48:10</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>10/15 (66.67%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Vanh Leg</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:48:23</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>13/15 (86.67%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:48:42</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>9/15 (60.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Vanh Leg</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:49:01</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>13/15 (86.67%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DinhNhatKy</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:49:34</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Ta Hoang Giang</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:50:10</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Nguyen Van Tinh</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:50:40</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>DinhNhatKy</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:51:01</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>13/15 (86.67%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:51:25</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0/15 (0.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Nguyen Van Tinh</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:51:38</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Nguyen Van Tinh</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:52:24</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>13/15 (86.67%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>NguyenHuuDuc</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:52:25</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>DinhNhatKy</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:52:45</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>NguyenHuuDuc</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:53:02</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Nguyen Van Tinh</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:53:25</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>sontung</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:55:26</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>sontung</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:55:39</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sontung</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:55:53</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>sontung</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:56:12</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Chi Dân</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:56:27</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Karik</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:57:00</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Karik</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2024-12-03 16:57:17</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>15/15 (100.00%)</t>
         </is>
       </c>
     </row>

</xml_diff>